<commit_message>
add new row ibrahim
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p\Desktop\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data analysis\bi sohag\Source Control\Day 2\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFCCB635-7129-4139-99E9-47036FBB8593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446A9134-A9DF-433A-86AA-B31399B00021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>aya</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>mohamed</t>
+  </si>
+  <si>
+    <t>ibrahim</t>
+  </si>
+  <si>
+    <t>29age</t>
   </si>
 </sst>
 </file>
@@ -56,7 +62,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -363,18 +369,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -390,7 +396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -398,12 +404,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>